<commit_message>
Perbarui Folder Penyimpanan & Contoh
</commit_message>
<xml_diff>
--- a/storage/app/contoh/statistik-sdm.xlsx
+++ b/storage/app/contoh/statistik-sdm.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>penempatan_no_absen</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>OS-DAN</t>
+  </si>
+  <si>
+    <t>0S-BLD</t>
   </si>
   <si>
     <t>OS-MKS</t>
@@ -437,18 +440,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd\ h:mm"/>
-    <numFmt numFmtId="181" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="mm"/>
-    <numFmt numFmtId="183" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="yyyy"/>
-    <numFmt numFmtId="185" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="yyyy\-mm\-dd\ h:mm"/>
+    <numFmt numFmtId="182" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="183" formatCode="mm"/>
+    <numFmt numFmtId="184" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="185" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -495,6 +498,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Roboto Medium"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -503,7 +519,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -525,7 +541,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,9 +561,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -563,61 +642,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -625,22 +650,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -661,7 +670,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +700,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,115 +790,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,19 +826,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,18 +844,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1207,6 +1216,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD8D8D8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD8D8D8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD8D8D8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFD8D8D8"/>
       </left>
       <right/>
@@ -1284,6 +1319,15 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF7F7F7F"/>
@@ -1307,17 +1351,57 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFD8D8D8"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFD8D8D8"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD8D8D8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD8D8D8"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD8D8D8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1344,6 +1428,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1391,152 +1490,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1544,7 +1643,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1586,13 +1685,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1601,43 +1700,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1649,34 +1748,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1697,16 +1796,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="185" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="185" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1715,16 +1814,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1745,40 +1844,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1799,83 +1904,107 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2270,7 +2399,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="17" max="17" width="9.14285714285714" style="113"/>
+    <col min="17" max="17" width="9.14285714285714" style="123"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -2322,7 +2451,7 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="113" t="s">
+      <c r="Q1" s="123" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
@@ -2363,9 +2492,9 @@
       </c>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
+      <c r="B2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2385,11 +2514,11 @@
   <dimension ref="A1:BF66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2413,7 +2542,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:46">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -2456,17 +2585,18 @@
       <c r="AJ3" s="7"/>
       <c r="AK3" s="7"/>
       <c r="AL3" s="59"/>
-      <c r="AM3" s="84" t="s">
+      <c r="AM3" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="AN3" s="85"/>
-      <c r="AO3" s="85"/>
-      <c r="AP3" s="85"/>
-      <c r="AQ3" s="85"/>
-      <c r="AR3" s="85"/>
-      <c r="AS3" s="101"/>
+      <c r="AN3" s="87"/>
+      <c r="AO3" s="87"/>
+      <c r="AP3" s="87"/>
+      <c r="AQ3" s="87"/>
+      <c r="AR3" s="87"/>
+      <c r="AS3" s="87"/>
+      <c r="AT3" s="106"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="14.25" customHeight="1" spans="1:45">
+    <row r="4" s="1" customFormat="1" ht="14.25" customHeight="1" spans="1:46">
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
@@ -2525,15 +2655,16 @@
       </c>
       <c r="AK4" s="69"/>
       <c r="AL4" s="69"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="87"/>
-      <c r="AS4" s="102"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="89"/>
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="107"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="84.75" customHeight="1" spans="1:46">
+    <row r="5" s="1" customFormat="1" ht="84.75" customHeight="1" spans="1:47">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>43</v>
@@ -2642,34 +2773,37 @@
       <c r="AL5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="AM5" s="88" t="s">
+      <c r="AM5" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="AN5" s="89" t="s">
+      <c r="AN5" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="AO5" s="89" t="s">
+      <c r="AO5" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="AP5" s="89" t="s">
+      <c r="AP5" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="AQ5" s="89" t="s">
+      <c r="AQ5" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="AR5" s="103" t="s">
+      <c r="AR5" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="AS5" s="104" t="s">
+      <c r="AS5" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="AT5" s="105" t="s">
+      <c r="AT5" s="111" t="s">
         <v>79</v>
       </c>
+      <c r="AU5" s="112" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:50">
       <c r="A6" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B6" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -2811,7 +2945,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK6" s="90">
+      <c r="AK6" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -2835,26 +2969,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ6" s="90">
+      <c r="AQ6" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR6" s="90">
+      <c r="AR6" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS6" s="18">
+      <c r="AS6" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT6" s="106">
-        <f t="shared" ref="AT6:AT15" si="0">SUM(AD6:AS6)</f>
-        <v>0</v>
-      </c>
+      <c r="AT6" s="18">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU6" s="113">
+        <f t="shared" ref="AU6:AU15" si="0">SUM(AD6:AT6)</f>
+        <v>0</v>
+      </c>
+      <c r="AX6" s="2"/>
     </row>
-    <row r="7" ht="16.5" customHeight="1" spans="1:46">
+    <row r="7" ht="16.5" customHeight="1" spans="1:50">
       <c r="A7" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B7" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -2996,7 +3135,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK7" s="90">
+      <c r="AK7" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3020,26 +3159,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ7" s="90">
+      <c r="AQ7" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR7" s="90">
+      <c r="AR7" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS7" s="18">
+      <c r="AS7" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="106">
+      <c r="AT7" s="18">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX7" s="2"/>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:50">
       <c r="A8" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B8" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -3181,7 +3325,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK8" s="90">
+      <c r="AK8" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3205,26 +3349,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ8" s="90">
+      <c r="AQ8" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR8" s="90">
+      <c r="AR8" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS8" s="18">
+      <c r="AS8" s="92">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT8" s="106">
+      <c r="AT8" s="18">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX8" s="2"/>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:50">
       <c r="A9" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -3366,7 +3515,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK9" s="91">
+      <c r="AK9" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3390,26 +3539,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ9" s="91">
+      <c r="AQ9" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR9" s="91">
+      <c r="AR9" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS9" s="57">
+      <c r="AS9" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT9" s="107">
+      <c r="AT9" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX9" s="2"/>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:50">
       <c r="A10" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B10" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -3551,7 +3705,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK10" s="91">
+      <c r="AK10" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3575,26 +3729,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ10" s="91">
+      <c r="AQ10" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR10" s="91">
+      <c r="AR10" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS10" s="57">
+      <c r="AS10" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT10" s="107">
+      <c r="AT10" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX10" s="2"/>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:50">
       <c r="A11" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B11" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -3736,7 +3895,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK11" s="91">
+      <c r="AK11" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3760,26 +3919,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ11" s="91">
+      <c r="AQ11" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR11" s="91">
+      <c r="AR11" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS11" s="57">
+      <c r="AS11" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT11" s="107">
+      <c r="AT11" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX11" s="2"/>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:50">
       <c r="A12" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B12" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -3921,7 +4085,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK12" s="91">
+      <c r="AK12" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -3945,26 +4109,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ12" s="91">
+      <c r="AQ12" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR12" s="91">
+      <c r="AR12" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS12" s="57">
+      <c r="AS12" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT12" s="107">
+      <c r="AT12" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX12" s="2"/>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:50">
       <c r="A13" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -4106,7 +4275,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK13" s="91">
+      <c r="AK13" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -4130,26 +4299,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ13" s="91">
+      <c r="AQ13" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR13" s="91">
+      <c r="AR13" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS13" s="57">
+      <c r="AS13" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT13" s="107">
+      <c r="AT13" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX13" s="2"/>
     </row>
-    <row r="14" ht="13.5" customHeight="1" spans="1:46">
+    <row r="14" ht="13.5" customHeight="1" spans="1:50">
       <c r="A14" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -4291,7 +4465,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK14" s="91">
+      <c r="AK14" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -4315,26 +4489,31 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ14" s="91">
+      <c r="AQ14" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR14" s="91">
+      <c r="AR14" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS14" s="57">
+      <c r="AS14" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT14" s="107">
+      <c r="AT14" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX14" s="2"/>
     </row>
-    <row r="15" ht="13.5" customHeight="1" spans="1:46">
+    <row r="15" ht="13.5" customHeight="1" spans="1:50">
       <c r="A15" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B15" s="17">
         <f>COUNTIFS(Penempatan[sdm_kelamin],B$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*")</f>
@@ -4460,7 +4639,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AF$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
         <v>0</v>
       </c>
-      <c r="AG15" s="92">
+      <c r="AG15" s="94">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AG$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AG$4)</f>
         <v>0</v>
       </c>
@@ -4472,11 +4651,11 @@
         <f>COUNTIFS(Penempatan[penempatan_kategori],AI$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AG$4)</f>
         <v>0</v>
       </c>
-      <c r="AJ15" s="92">
+      <c r="AJ15" s="94">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AJ$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
-      <c r="AK15" s="91">
+      <c r="AK15" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kategori],AK$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AJ$4)</f>
         <v>0</v>
       </c>
@@ -4500,24 +4679,29 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AP$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AQ15" s="91">
+      <c r="AQ15" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AQ$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AR15" s="91">
+      <c r="AR15" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AR$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AS15" s="57">
+      <c r="AS15" s="93">
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AS$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AT15" s="107">
+      <c r="AT15" s="57">
+        <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="114">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AX15" s="2"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1" spans="1:46">
+    <row r="16" ht="13.5" customHeight="1" spans="1:50">
       <c r="A16" s="21"/>
       <c r="B16" s="22">
         <f t="shared" ref="B16:AT16" si="1">SUM(B6:B15)</f>
@@ -4659,7 +4843,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK16" s="93">
+      <c r="AK16" s="95">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4667,40 +4851,45 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AM16" s="94">
+      <c r="AM16" s="96">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN16" s="95">
+      <c r="AN16" s="97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="95">
+      <c r="AO16" s="97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AP16" s="26">
+      <c r="AP16" s="97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AQ16" s="93">
+      <c r="AQ16" s="115">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AR16" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AS16" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AT16" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="AR16" s="115">
+        <f>SUM(AR6:AR15)</f>
+        <v>0</v>
+      </c>
+      <c r="AS16" s="115">
+        <f>SUM(AS6:AS15)</f>
+        <v>0</v>
+      </c>
+      <c r="AT16" s="116">
+        <f>SUM(AT6:AT15)</f>
+        <v>0</v>
+      </c>
+      <c r="AU16" s="24">
+        <f>SUM(AU6:AU15)</f>
+        <v>0</v>
+      </c>
+      <c r="AX16" s="2"/>
     </row>
-    <row r="17" spans="2:45">
+    <row r="17" spans="2:46">
       <c r="B17" s="27">
         <f>SUM(B16:C16)</f>
         <v>0</v>
@@ -4757,20 +4946,21 @@
         <f>SUM(AJ16:AL16)</f>
         <v>0</v>
       </c>
-      <c r="AK17" s="96"/>
-      <c r="AL17" s="97"/>
-      <c r="AM17" s="98">
-        <f>SUM(AM16:AS16)</f>
-        <v>0</v>
-      </c>
-      <c r="AN17" s="99"/>
-      <c r="AO17" s="99"/>
-      <c r="AP17" s="99"/>
-      <c r="AQ17" s="99"/>
-      <c r="AR17" s="99"/>
-      <c r="AS17" s="108"/>
+      <c r="AK17" s="98"/>
+      <c r="AL17" s="99"/>
+      <c r="AM17" s="100">
+        <f>SUM(AM16:AT16)</f>
+        <v>0</v>
+      </c>
+      <c r="AN17" s="101"/>
+      <c r="AO17" s="101"/>
+      <c r="AP17" s="101"/>
+      <c r="AQ17" s="101"/>
+      <c r="AR17" s="101"/>
+      <c r="AS17" s="101"/>
+      <c r="AT17" s="117"/>
     </row>
-    <row r="18" spans="2:45">
+    <row r="18" spans="2:46">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
@@ -4799,30 +4989,31 @@
       <c r="AA18" s="29"/>
       <c r="AB18" s="29"/>
       <c r="AC18" s="29"/>
-      <c r="AD18" s="27">
+      <c r="AD18" s="77">
         <f>SUM(AD17:AL17)</f>
         <v>0</v>
       </c>
-      <c r="AE18" s="77"/>
-      <c r="AF18" s="30"/>
-      <c r="AG18" s="30"/>
-      <c r="AH18" s="30"/>
-      <c r="AI18" s="30"/>
-      <c r="AJ18" s="30"/>
-      <c r="AK18" s="100"/>
-      <c r="AL18" s="28"/>
-      <c r="AM18" s="78">
+      <c r="AE18" s="78"/>
+      <c r="AF18" s="79"/>
+      <c r="AG18" s="79"/>
+      <c r="AH18" s="79"/>
+      <c r="AI18" s="79"/>
+      <c r="AJ18" s="79"/>
+      <c r="AK18" s="102"/>
+      <c r="AL18" s="103"/>
+      <c r="AM18" s="104">
         <f>SUM(AM17)</f>
         <v>0</v>
       </c>
-      <c r="AN18" s="79"/>
-      <c r="AO18" s="79"/>
-      <c r="AP18" s="79"/>
-      <c r="AQ18" s="79"/>
-      <c r="AR18" s="79"/>
-      <c r="AS18" s="109"/>
+      <c r="AN18" s="105"/>
+      <c r="AO18" s="105"/>
+      <c r="AP18" s="105"/>
+      <c r="AQ18" s="105"/>
+      <c r="AR18" s="105"/>
+      <c r="AS18" s="105"/>
+      <c r="AT18" s="118"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:46">
       <c r="A19" s="4"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -4852,34 +5043,35 @@
       <c r="AA19" s="29"/>
       <c r="AB19" s="29"/>
       <c r="AC19" s="29"/>
-      <c r="AD19" s="78">
+      <c r="AD19" s="80">
         <f>SUM(AD18:AS18)</f>
         <v>0</v>
       </c>
-      <c r="AE19" s="79"/>
-      <c r="AF19" s="79"/>
-      <c r="AG19" s="79"/>
-      <c r="AH19" s="79"/>
-      <c r="AI19" s="79"/>
-      <c r="AJ19" s="79"/>
-      <c r="AK19" s="79"/>
-      <c r="AL19" s="79"/>
-      <c r="AM19" s="79"/>
-      <c r="AN19" s="79"/>
-      <c r="AO19" s="79"/>
-      <c r="AP19" s="79"/>
-      <c r="AQ19" s="79"/>
-      <c r="AR19" s="79"/>
-      <c r="AS19" s="109"/>
+      <c r="AE19" s="81"/>
+      <c r="AF19" s="81"/>
+      <c r="AG19" s="81"/>
+      <c r="AH19" s="81"/>
+      <c r="AI19" s="81"/>
+      <c r="AJ19" s="81"/>
+      <c r="AK19" s="81"/>
+      <c r="AL19" s="81"/>
+      <c r="AM19" s="81"/>
+      <c r="AN19" s="81"/>
+      <c r="AO19" s="81"/>
+      <c r="AP19" s="81"/>
+      <c r="AQ19" s="81"/>
+      <c r="AR19" s="81"/>
+      <c r="AS19" s="81"/>
+      <c r="AT19" s="119"/>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" ht="15.75" spans="1:49">
       <c r="A23" s="31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" s="6" t="str">
         <f ca="1">"ORGANIK "&amp;YEAR(B24)</f>
@@ -4942,12 +5134,12 @@
       <c r="AV23" s="7"/>
       <c r="AW23" s="59"/>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" ht="16.5" spans="1:49">
       <c r="A24" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" s="33">
-        <f ca="1" t="shared" ref="B24:X24" si="2">Z24</f>
+        <f ca="1" t="shared" ref="B24:Y24" si="2">Z24</f>
         <v>44562</v>
       </c>
       <c r="C24" s="34">
@@ -5039,7 +5231,7 @@
         <v>45231</v>
       </c>
       <c r="Y24" s="60">
-        <f ca="1">AW24</f>
+        <f ca="1" t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="Z24" s="61">
@@ -5139,7 +5331,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" ht="15.75" spans="1:49">
       <c r="A25" s="35" t="s">
         <v>30</v>
       </c>
@@ -5195,21 +5387,21 @@
         <f ca="1">IF(N24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(N$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(N$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(N$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="O25" s="19" t="str">
+      <c r="O25" s="19">
         <f ca="1">IF(O24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(O$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(O$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(O$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="P25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="P25" s="19">
         <f ca="1">IF(P24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(P$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(P$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(P$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="19">
         <f ca="1">IF(Q24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Q$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Q$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(Q$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="R25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="R25" s="19">
         <f ca="1">IF(R24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(R$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(R$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(R$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S25" s="19" t="str">
         <f ca="1">IF(S24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(S$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(S$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(S$24,1),Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5291,21 +5483,21 @@
         <f ca="1">IF(AL24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AL$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AL$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AL$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="AM25" s="19" t="str">
+      <c r="AM25" s="19">
         <f ca="1">IF(AM24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AM$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AM$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AM$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AN25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="19">
         <f ca="1">IF(AN24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AN$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AN$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AN$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AO25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AO25" s="19">
         <f ca="1">IF(AO24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AO$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AO$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AO$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AP25" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AP25" s="19">
         <f ca="1">IF(AP24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AP$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AP$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AP$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AQ25" s="19" t="str">
         <f ca="1">IF(AQ24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AQ$24,1),Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24)+COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(AQ$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;EDATE(AQ$24,1),Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5338,7 +5530,7 @@
     </row>
     <row r="26" spans="1:49">
       <c r="A26" s="36" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B26" s="17">
         <f ca="1">IF(B24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!B$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!B$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5392,21 +5584,21 @@
         <f ca="1">IF(N24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!N$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!N$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="O26" s="19" t="str">
+      <c r="O26" s="19">
         <f ca="1">IF(O24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!O$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!O$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="P26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="P26" s="19">
         <f ca="1">IF(P24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!P$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!P$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="19">
         <f ca="1">IF(Q24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!Q$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!Q$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="R26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="R26" s="19">
         <f ca="1">IF(R24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!R$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!R$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S26" s="19" t="str">
         <f ca="1">IF(S24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!S$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!S$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5488,21 +5680,21 @@
         <f ca="1">IF(AL24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AL$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AL$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="AM26" s="19" t="str">
+      <c r="AM26" s="19">
         <f ca="1">IF(AM24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AM$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AM$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AN26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="19">
         <f ca="1">IF(AN24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AN$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AN$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AO26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="19">
         <f ca="1">IF(AO24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AO$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AO$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AP26" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="19">
         <f ca="1">IF(AP24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AP$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AP$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AQ26" s="19" t="str">
         <f ca="1">IF(AQ24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_gabung],"&lt;"&amp;EDATE(Sum!AQ$24,1),Penempatan[sdm_tgl_gabung],"&gt;="&amp;Sum!AQ$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5535,7 +5727,7 @@
     </row>
     <row r="27" ht="13.5" customHeight="1" spans="1:49">
       <c r="A27" s="37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B27" s="38">
         <f ca="1">IF(B24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!B$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!B$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5589,21 +5781,21 @@
         <f ca="1">IF(N24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!N$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!N$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="O27" s="39" t="str">
+      <c r="O27" s="39">
         <f ca="1">IF(O24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!O$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!O$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="P27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="P27" s="39">
         <f ca="1">IF(P24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!P$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!P$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="39">
         <f ca="1">IF(Q24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!Q$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!Q$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="R27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="R27" s="39">
         <f ca="1">IF(R24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!R$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!R$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S27" s="39" t="str">
         <f ca="1">IF(S24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!S$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!S$24,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5685,21 +5877,21 @@
         <f ca="1">IF(AL24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AL$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AL$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
         <v>0</v>
       </c>
-      <c r="AM27" s="39" t="str">
+      <c r="AM27" s="39">
         <f ca="1">IF(AM24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AM$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AM$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AN27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="39">
         <f ca="1">IF(AN24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AN$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AN$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AO27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="39">
         <f ca="1">IF(AO24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AO$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AO$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
-      </c>
-      <c r="AP27" s="39" t="str">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="39">
         <f ca="1">IF(AP24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AP$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AP$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AQ27" s="39" t="str">
         <f ca="1">IF(AQ24&gt;TODAY(),"",COUNTIFS(Penempatan[sdm_tgl_berhenti],"&lt;"&amp;EDATE(Sum!AQ$24,1),Penempatan[sdm_tgl_berhenti],"&gt;="&amp;Sum!AQ$24,Penempatan[penempatan_kontrak],"=OS-*",Penempatan[penempatan_lokasi],$A$24))</f>
@@ -5732,7 +5924,7 @@
     </row>
     <row r="28" ht="13.5" customHeight="1" spans="1:49">
       <c r="A28" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B28" s="41" t="str">
         <f ca="1" t="shared" ref="B28:AW28" si="4">IFERROR((B27/AVERAGE(B25-B26,B25+B27))*100,"")</f>
@@ -5929,7 +6121,7 @@
     </row>
     <row r="29" ht="13.5" customHeight="1" spans="1:49">
       <c r="A29" s="43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B29" s="44" t="str">
         <f ca="1">IFERROR(AVERAGE(B28:M28),"")</f>
@@ -6056,7 +6248,7 @@
     </row>
     <row r="33" spans="2:58">
       <c r="B33" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -6067,7 +6259,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="10"/>
       <c r="K33" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
@@ -6078,7 +6270,7 @@
       <c r="R33" s="13"/>
       <c r="S33" s="10"/>
       <c r="T33" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
@@ -6089,7 +6281,7 @@
       <c r="AA33" s="13"/>
       <c r="AB33" s="10"/>
       <c r="AC33" s="69" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AD33" s="69"/>
       <c r="AE33" s="69"/>
@@ -6097,7 +6289,7 @@
       <c r="AG33" s="69"/>
       <c r="AH33" s="69"/>
       <c r="AI33" s="69" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AJ33" s="69"/>
       <c r="AK33" s="69"/>
@@ -6105,7 +6297,7 @@
       <c r="AM33" s="69"/>
       <c r="AN33" s="69"/>
       <c r="AO33" s="69" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AP33" s="69"/>
       <c r="AQ33" s="69"/>
@@ -6124,10 +6316,10 @@
     </row>
     <row r="34" spans="1:58">
       <c r="A34" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="49"/>
@@ -6138,7 +6330,7 @@
       <c r="I34" s="49"/>
       <c r="J34" s="64"/>
       <c r="K34" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L34" s="49"/>
       <c r="M34" s="49"/>
@@ -6149,7 +6341,7 @@
       <c r="R34" s="49"/>
       <c r="S34" s="64"/>
       <c r="T34" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="U34" s="49"/>
       <c r="V34" s="49"/>
@@ -6159,30 +6351,30 @@
       <c r="Z34" s="49"/>
       <c r="AA34" s="49"/>
       <c r="AB34" s="64"/>
-      <c r="AC34" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="AD34" s="80"/>
-      <c r="AE34" s="80"/>
-      <c r="AF34" s="80"/>
-      <c r="AG34" s="80"/>
-      <c r="AH34" s="80"/>
-      <c r="AI34" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ34" s="80"/>
-      <c r="AK34" s="80"/>
-      <c r="AL34" s="80"/>
-      <c r="AM34" s="80"/>
-      <c r="AN34" s="80"/>
-      <c r="AO34" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="AP34" s="80"/>
-      <c r="AQ34" s="80"/>
-      <c r="AR34" s="80"/>
-      <c r="AS34" s="80"/>
-      <c r="AT34" s="80"/>
+      <c r="AC34" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD34" s="82"/>
+      <c r="AE34" s="82"/>
+      <c r="AF34" s="82"/>
+      <c r="AG34" s="82"/>
+      <c r="AH34" s="82"/>
+      <c r="AI34" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ34" s="82"/>
+      <c r="AK34" s="82"/>
+      <c r="AL34" s="82"/>
+      <c r="AM34" s="82"/>
+      <c r="AN34" s="82"/>
+      <c r="AO34" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP34" s="82"/>
+      <c r="AQ34" s="82"/>
+      <c r="AR34" s="82"/>
+      <c r="AS34" s="82"/>
+      <c r="AT34" s="82"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
       <c r="AZ34" s="2"/>
@@ -6222,7 +6414,7 @@
         <v>24</v>
       </c>
       <c r="J35" s="56" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K35" s="50">
         <v>1</v>
@@ -6249,7 +6441,7 @@
         <v>24</v>
       </c>
       <c r="S35" s="56" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T35" s="50">
         <v>1</v>
@@ -6276,7 +6468,7 @@
         <v>24</v>
       </c>
       <c r="AB35" s="56" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AC35" s="50">
         <v>18</v>
@@ -6294,7 +6486,7 @@
         <v>57</v>
       </c>
       <c r="AH35" s="56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AI35" s="50">
         <v>18</v>
@@ -6312,7 +6504,7 @@
         <v>57</v>
       </c>
       <c r="AN35" s="56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AO35" s="50">
         <v>18</v>
@@ -6330,7 +6522,7 @@
         <v>57</v>
       </c>
       <c r="AT35" s="56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
@@ -6344,7 +6536,7 @@
     </row>
     <row r="36" spans="1:58">
       <c r="A36" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B36" s="17">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A36,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -6538,7 +6730,7 @@
     </row>
     <row r="37" spans="1:58">
       <c r="A37" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="17">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A37,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -6732,7 +6924,7 @@
     </row>
     <row r="38" spans="1:58">
       <c r="A38" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" s="17">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A38,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -6926,7 +7118,7 @@
     </row>
     <row r="39" spans="1:58">
       <c r="A39" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A39,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -7120,7 +7312,7 @@
     </row>
     <row r="40" spans="1:58">
       <c r="A40" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A40,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -7314,7 +7506,7 @@
     </row>
     <row r="41" spans="1:58">
       <c r="A41" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A41,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -7508,7 +7700,7 @@
     </row>
     <row r="42" spans="1:58">
       <c r="A42" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A42,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -7702,7 +7894,7 @@
     </row>
     <row r="43" spans="1:58">
       <c r="A43" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A43,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -7896,7 +8088,7 @@
     </row>
     <row r="44" spans="1:58">
       <c r="A44" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B44" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A44,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -8090,7 +8282,7 @@
     </row>
     <row r="45" ht="13.5" customHeight="1" spans="1:58">
       <c r="A45" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="38">
         <f>COUNTIFS(Penempatan[masa_kerja],"",Penempatan[penempatan_lokasi],$A45,Penempatan[sdm_tgl_berhenti],"",Penempatan[penempatan_kontrak],$AD$4)</f>
@@ -8511,33 +8703,33 @@
       <c r="Z47" s="30"/>
       <c r="AA47" s="30"/>
       <c r="AB47" s="28"/>
-      <c r="AC47" s="81">
+      <c r="AC47" s="83">
         <f>SUM(AC46:AH46)</f>
         <v>0</v>
       </c>
-      <c r="AD47" s="81"/>
-      <c r="AE47" s="81"/>
-      <c r="AF47" s="81"/>
-      <c r="AG47" s="81"/>
-      <c r="AH47" s="81"/>
-      <c r="AI47" s="81">
+      <c r="AD47" s="83"/>
+      <c r="AE47" s="83"/>
+      <c r="AF47" s="83"/>
+      <c r="AG47" s="83"/>
+      <c r="AH47" s="83"/>
+      <c r="AI47" s="83">
         <f>SUM(AI46:AN46)</f>
         <v>0</v>
       </c>
-      <c r="AJ47" s="81"/>
-      <c r="AK47" s="81"/>
-      <c r="AL47" s="81"/>
-      <c r="AM47" s="81"/>
-      <c r="AN47" s="81"/>
-      <c r="AO47" s="81">
+      <c r="AJ47" s="83"/>
+      <c r="AK47" s="83"/>
+      <c r="AL47" s="83"/>
+      <c r="AM47" s="83"/>
+      <c r="AN47" s="83"/>
+      <c r="AO47" s="83">
         <f>SUM(AO46:AT46)</f>
         <v>0</v>
       </c>
-      <c r="AP47" s="81"/>
-      <c r="AQ47" s="81"/>
-      <c r="AR47" s="81"/>
-      <c r="AS47" s="81"/>
-      <c r="AT47" s="81"/>
+      <c r="AP47" s="83"/>
+      <c r="AQ47" s="83"/>
+      <c r="AR47" s="83"/>
+      <c r="AS47" s="83"/>
+      <c r="AT47" s="83"/>
       <c r="AX47" s="2"/>
       <c r="AY47" s="2"/>
       <c r="AZ47" s="2"/>
@@ -8551,7 +8743,7 @@
     <row r="48" spans="1:58">
       <c r="A48" s="4"/>
       <c r="B48" s="52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C48" s="52"/>
       <c r="D48" s="52"/>
@@ -8565,7 +8757,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K48" s="66" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L48" s="67"/>
       <c r="M48" s="67"/>
@@ -8579,7 +8771,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T48" s="66" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U48" s="67"/>
       <c r="V48" s="67"/>
@@ -8592,35 +8784,35 @@
         <f>AVERAGEIFS(Penempatan[masa_kerja],Penempatan[penempatan_kontrak],"=OS-*",Penempatan[sdm_tgl_berhenti],"")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC48" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="AD48" s="83"/>
-      <c r="AE48" s="83"/>
-      <c r="AF48" s="83"/>
-      <c r="AG48" s="83"/>
+      <c r="AC48" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD48" s="85"/>
+      <c r="AE48" s="85"/>
+      <c r="AF48" s="85"/>
+      <c r="AG48" s="85"/>
       <c r="AH48" s="65" t="e">
         <f>AVERAGEIFS(Penempatan[usia],Penempatan[penempatan_kontrak],$AD$4,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI48" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ48" s="83"/>
-      <c r="AK48" s="83"/>
-      <c r="AL48" s="83"/>
-      <c r="AM48" s="83"/>
+      <c r="AI48" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ48" s="85"/>
+      <c r="AK48" s="85"/>
+      <c r="AL48" s="85"/>
+      <c r="AM48" s="85"/>
       <c r="AN48" s="65" t="e">
         <f>AVERAGEIFS(Penempatan[usia],Penempatan[penempatan_kontrak],"&lt;&gt;PKWTT",Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AO48" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="AP48" s="83"/>
-      <c r="AQ48" s="83"/>
-      <c r="AR48" s="83"/>
-      <c r="AS48" s="83"/>
+      <c r="AO48" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP48" s="85"/>
+      <c r="AQ48" s="85"/>
+      <c r="AR48" s="85"/>
+      <c r="AS48" s="85"/>
       <c r="AT48" s="65" t="e">
         <f>AVERAGEIFS(Penempatan[usia],Penempatan[penempatan_kontrak],"=OS-*",Penempatan[sdm_tgl_berhenti],"")</f>
         <v>#DIV/0!</v>
@@ -8775,12 +8967,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" spans="1:5">
       <c r="A53" s="31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B53" s="54">
         <f ca="1">EDATE(D53,-12)</f>
@@ -8795,16 +8987,16 @@
     </row>
     <row r="54" ht="16.5" customHeight="1" spans="1:5">
       <c r="A54" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" s="56" t="s">
         <v>32</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E54" s="56" t="s">
         <v>32</v>
@@ -8812,7 +9004,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1" spans="1:5">
       <c r="A55" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B55" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A55,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8833,7 +9025,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B56" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A56,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8854,7 +9046,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B57" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A57,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8875,7 +9067,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B58" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A58,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8896,7 +9088,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B59" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A59,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8917,7 +9109,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B60" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A60,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8938,7 +9130,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B61" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A61,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8959,7 +9151,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B62" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A62,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -8980,7 +9172,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B63" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A63,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -9001,7 +9193,7 @@
     </row>
     <row r="64" ht="13.5" customHeight="1" spans="1:5">
       <c r="A64" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B64" s="17">
         <f ca="1">COUNTIFS(Penempatan[sdm_jenis_berhenti],$A64,Penempatan[penempatan_lokasi],$A$54,Penempatan[penempatan_kontrak],"&lt;&gt;OS-*",Penempatan[sdm_tgl_berhenti],"&gt;"&amp;$B$53,Penempatan[sdm_tgl_berhenti],"&lt;="&amp;EDATE($B$53,12))</f>
@@ -9022,19 +9214,19 @@
     </row>
     <row r="65" ht="13.5" customHeight="1" spans="1:5">
       <c r="A65" s="21"/>
-      <c r="B65" s="110">
+      <c r="B65" s="120">
         <f ca="1">SUM(B55:B64)</f>
         <v>0</v>
       </c>
-      <c r="C65" s="111">
+      <c r="C65" s="121">
         <f ca="1">SUM(C55:C64)</f>
         <v>0</v>
       </c>
-      <c r="D65" s="110">
+      <c r="D65" s="120">
         <f ca="1">SUM(D55:D64)</f>
         <v>0</v>
       </c>
-      <c r="E65" s="111">
+      <c r="E65" s="121">
         <f ca="1">SUM(E55:E64)</f>
         <v>0</v>
       </c>
@@ -9044,12 +9236,12 @@
         <f ca="1">SUM(B65:C65)</f>
         <v>0</v>
       </c>
-      <c r="C66" s="112"/>
+      <c r="C66" s="122"/>
       <c r="D66" s="27">
         <f ca="1">SUM(D65:E65)</f>
         <v>0</v>
       </c>
-      <c r="E66" s="112"/>
+      <c r="E66" s="122"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -9069,10 +9261,10 @@
     <mergeCell ref="AD17:AF17"/>
     <mergeCell ref="AG17:AI17"/>
     <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="AM17:AS17"/>
+    <mergeCell ref="AM17:AT17"/>
     <mergeCell ref="AD18:AL18"/>
-    <mergeCell ref="AM18:AS18"/>
-    <mergeCell ref="AD19:AS19"/>
+    <mergeCell ref="AM18:AT18"/>
+    <mergeCell ref="AD19:AT19"/>
     <mergeCell ref="B23:M23"/>
     <mergeCell ref="N23:Y23"/>
     <mergeCell ref="Z23:AK23"/>
@@ -9112,7 +9304,7 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="AM3:AS4"/>
+    <mergeCell ref="AM3:AT4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24 A54">

</xml_diff>

<commit_message>
Perbaiki Kesalahan Judul Data Contoh
</commit_message>
<xml_diff>
--- a/storage/app/contoh/statistik-sdm.xlsx
+++ b/storage/app/contoh/statistik-sdm.xlsx
@@ -248,7 +248,7 @@
     <t>OS-DAN</t>
   </si>
   <si>
-    <t>0S-BLD</t>
+    <t>OS-BLD</t>
   </si>
   <si>
     <t>OS-MKS</t>
@@ -443,13 +443,13 @@
     <numFmt numFmtId="176" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="yyyy\-mm\-dd\ h:mm"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd\ h:mm"/>
+    <numFmt numFmtId="181" formatCode="mm"/>
     <numFmt numFmtId="182" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="183" formatCode="mm"/>
-    <numFmt numFmtId="184" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="yyyy"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="184" formatCode="yyyy"/>
+    <numFmt numFmtId="185" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -505,6 +505,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -513,6 +543,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -527,76 +580,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -608,17 +594,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -640,6 +618,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -649,7 +649,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -670,7 +670,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +700,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,31 +790,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,127 +850,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1408,6 +1408,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1417,17 +1437,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1447,17 +1473,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1472,170 +1487,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="49" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1643,7 +1643,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1733,10 +1733,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1757,25 +1757,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1796,10 +1796,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1814,16 +1814,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1964,14 +1964,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="182" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2004,7 +2001,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2399,7 +2396,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="17" max="17" width="9.14285714285714" style="123"/>
+    <col min="17" max="17" width="9.14285714285714" style="122"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -2451,7 +2448,7 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="123" t="s">
+      <c r="Q1" s="122" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
@@ -2492,9 +2489,9 @@
       </c>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
+      <c r="B2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2514,11 +2511,11 @@
   <dimension ref="A1:BF66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AP9" sqref="AP9"/>
+      <selection pane="bottomRight" activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2791,13 +2788,13 @@
       <c r="AR5" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="AS5" s="110" t="s">
+      <c r="AS5" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="AT5" s="111" t="s">
+      <c r="AT5" s="110" t="s">
         <v>79</v>
       </c>
-      <c r="AU5" s="112" t="s">
+      <c r="AU5" s="111" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2985,7 +2982,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A6,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU6" s="113">
+      <c r="AU6" s="112">
         <f t="shared" ref="AU6:AU15" si="0">SUM(AD6:AT6)</f>
         <v>0</v>
       </c>
@@ -3175,7 +3172,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A7,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="113">
+      <c r="AU7" s="112">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3365,7 +3362,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A8,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU8" s="113">
+      <c r="AU8" s="112">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3555,7 +3552,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A9,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU9" s="114">
+      <c r="AU9" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3745,7 +3742,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A10,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU10" s="114">
+      <c r="AU10" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3935,7 +3932,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A11,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU11" s="114">
+      <c r="AU11" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4125,7 +4122,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A12,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU12" s="114">
+      <c r="AU12" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4315,7 +4312,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A13,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU13" s="114">
+      <c r="AU13" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4505,7 +4502,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A14,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU14" s="114">
+      <c r="AU14" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4695,7 +4692,7 @@
         <f>COUNTIFS(Penempatan[penempatan_kontrak],AT$5,Penempatan[penempatan_lokasi],$A15,Penempatan[sdm_tgl_berhenti],"")</f>
         <v>0</v>
       </c>
-      <c r="AU15" s="114">
+      <c r="AU15" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4704,7 +4701,7 @@
     <row r="16" ht="13.5" customHeight="1" spans="1:50">
       <c r="A16" s="21"/>
       <c r="B16" s="22">
-        <f t="shared" ref="B16:AT16" si="1">SUM(B6:B15)</f>
+        <f t="shared" ref="B16:AU16" si="1">SUM(B6:B15)</f>
         <v>0</v>
       </c>
       <c r="C16" s="23">
@@ -4867,24 +4864,24 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AQ16" s="115">
+      <c r="AQ16" s="114">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AR16" s="115">
-        <f>SUM(AR6:AR15)</f>
-        <v>0</v>
-      </c>
-      <c r="AS16" s="115">
-        <f>SUM(AS6:AS15)</f>
-        <v>0</v>
-      </c>
-      <c r="AT16" s="116">
-        <f>SUM(AT6:AT15)</f>
+      <c r="AR16" s="114">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AS16" s="114">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT16" s="115">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU16" s="24">
-        <f>SUM(AU6:AU15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX16" s="2"/>
@@ -4958,7 +4955,7 @@
       <c r="AQ17" s="101"/>
       <c r="AR17" s="101"/>
       <c r="AS17" s="101"/>
-      <c r="AT17" s="117"/>
+      <c r="AT17" s="116"/>
     </row>
     <row r="18" spans="2:46">
       <c r="B18" s="29"/>
@@ -5011,7 +5008,7 @@
       <c r="AQ18" s="105"/>
       <c r="AR18" s="105"/>
       <c r="AS18" s="105"/>
-      <c r="AT18" s="118"/>
+      <c r="AT18" s="117"/>
     </row>
     <row r="19" spans="1:46">
       <c r="A19" s="4"/>
@@ -5062,7 +5059,7 @@
       <c r="AQ19" s="81"/>
       <c r="AR19" s="81"/>
       <c r="AS19" s="81"/>
-      <c r="AT19" s="119"/>
+      <c r="AT19" s="118"/>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
@@ -9214,19 +9211,19 @@
     </row>
     <row r="65" ht="13.5" customHeight="1" spans="1:5">
       <c r="A65" s="21"/>
-      <c r="B65" s="120">
+      <c r="B65" s="119">
         <f ca="1">SUM(B55:B64)</f>
         <v>0</v>
       </c>
-      <c r="C65" s="121">
+      <c r="C65" s="120">
         <f ca="1">SUM(C55:C64)</f>
         <v>0</v>
       </c>
-      <c r="D65" s="120">
+      <c r="D65" s="119">
         <f ca="1">SUM(D55:D64)</f>
         <v>0</v>
       </c>
-      <c r="E65" s="121">
+      <c r="E65" s="120">
         <f ca="1">SUM(E55:E64)</f>
         <v>0</v>
       </c>
@@ -9236,12 +9233,12 @@
         <f ca="1">SUM(B65:C65)</f>
         <v>0</v>
       </c>
-      <c r="C66" s="122"/>
+      <c r="C66" s="121"/>
       <c r="D66" s="27">
         <f ca="1">SUM(D65:E65)</f>
         <v>0</v>
       </c>
-      <c r="E66" s="122"/>
+      <c r="E66" s="121"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>